<commit_message>
added redmi, other fixes
</commit_message>
<xml_diff>
--- a/my_project/output_result_data/calc_correlations_result_data/corr_binding_approach_results.xlsx
+++ b/my_project/output_result_data/calc_correlations_result_data/corr_binding_approach_results.xlsx
@@ -457,13 +457,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9999999865138811</v>
+        <v>-0.2706454968469449</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9897433186107869</v>
+        <v>-0.1107188520745969</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.2164895428247857</v>
       </c>
     </row>
     <row r="3">
@@ -473,13 +473,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.000104553509040095</v>
+        <v>0.009071768512644917</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0912578966859804</v>
+        <v>0.2933999403716067</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.03819527810955458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>